<commit_message>
Fix errors in phage-genomes in supp_tables. Accession numbers don't allow ENTREY query.
</commit_message>
<xml_diff>
--- a/docs/supplementary-tables.xlsx
+++ b/docs/supplementary-tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/PhiLab/Shared Documents/General/Papers in preparation/LC53 modification and CRISPR/CHM Revision Nov 2024/bioinformatics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://otagouni.sharepoint.com/sites/PhiLab/Shared Documents/General/Papers in preparation/LC53 modification and CRISPR/CHM Revision Nov 2024/bioinformatics/arabinosylation-anti-CRISPR/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="8_{3A860D05-BA79-4930-9466-171EFD6FED12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECE3628C-7E0F-4985-9D5F-461A01E5D0B4}"/>
+  <xr:revisionPtr revIDLastSave="337" documentId="8_{3A860D05-BA79-4930-9466-171EFD6FED12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9229572-EACA-4AA2-BE7F-93E87736A36C}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{F9CE20F1-D66E-494F-B2B1-7A22917EC080}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{F9CE20F1-D66E-494F-B2B1-7A22917EC080}"/>
   </bookViews>
   <sheets>
     <sheet name="S4_phages" sheetId="1" r:id="rId1"/>
@@ -1905,9 +1905,6 @@
     </r>
   </si>
   <si>
-    <t>MT385367</t>
-  </si>
-  <si>
     <r>
       <t>Acinetobacter</t>
     </r>
@@ -3322,13 +3319,16 @@
   </si>
   <si>
     <t>QPI17269.1</t>
+  </si>
+  <si>
+    <t>MT385367.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3376,13 +3376,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF3A7C22"/>
       <name val="Arial"/>
@@ -3422,7 +3415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3443,37 +3436,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3481,43 +3450,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3659,8 +3591,45 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -3679,7 +3648,26 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -3708,7 +3696,7 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i/>
+        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -3746,25 +3734,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
         <i/>
         <strike val="0"/>
         <condense val="0"/>
@@ -3775,82 +3744,6 @@
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -4034,6 +3927,82 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4176,12 +4145,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9858EA03-D35A-4C3C-A9DE-56BA4D6C0C61}" name="Table4" displayName="Table4" ref="A1:D36" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9858EA03-D35A-4C3C-A9DE-56BA4D6C0C61}" name="Table4" displayName="Table4" ref="A1:D36" totalsRowShown="0" headerRowDxfId="28">
   <autoFilter ref="A1:D36" xr:uid="{9858EA03-D35A-4C3C-A9DE-56BA4D6C0C61}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{74817D5F-4131-4081-A863-B086F9187AFA}" name="Species" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{C97A4734-EA5B-47F2-9601-3931FB777387}" name="Accession" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{817FC218-A528-4676-9F37-9CB414AAE1F7}" name="Genome size (bp)" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{74817D5F-4131-4081-A863-B086F9187AFA}" name="Species" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C97A4734-EA5B-47F2-9601-3931FB777387}" name="Accession" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{817FC218-A528-4676-9F37-9CB414AAE1F7}" name="Genome size (bp)" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{F01D5EE0-EB09-4BD9-9097-0DA63D88F05A}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4189,39 +4158,39 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5F127FE-2A3C-4A5A-8431-296D1263EC2D}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27" tableBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5F127FE-2A3C-4A5A-8431-296D1263EC2D}" name="Table1" displayName="Table1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A1:F7" xr:uid="{A5F127FE-2A3C-4A5A-8431-296D1263EC2D}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{65467636-A166-4E19-87F4-1B960C29EC64}" name="Species" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{9555FAEF-CEE9-4839-A7F8-4C55689C24DF}" name="Strain" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{4CA18E0D-1A70-4088-8E32-0BDE9001ABD6}" name="Accession" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{253923B9-8982-4FCE-BB80-2AA9BF5EB9AB}" name="Description" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{2E9EBB52-16CD-4A50-B51B-6772217E6C9B}" name="Notes" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{77A2DC02-CFF8-4D04-9E04-80FD29DDD00B}" name="Reference" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{65467636-A166-4E19-87F4-1B960C29EC64}" name="Species" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{9555FAEF-CEE9-4839-A7F8-4C55689C24DF}" name="Strain" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4CA18E0D-1A70-4088-8E32-0BDE9001ABD6}" name="Accession" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{253923B9-8982-4FCE-BB80-2AA9BF5EB9AB}" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{2E9EBB52-16CD-4A50-B51B-6772217E6C9B}" name="Notes" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{77A2DC02-CFF8-4D04-9E04-80FD29DDD00B}" name="Reference" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3A3A890D-49EE-4770-A722-1CC87E690383}" name="Table5" displayName="Table5" ref="A1:C43" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3A3A890D-49EE-4770-A722-1CC87E690383}" name="Table5" displayName="Table5" ref="A1:C43" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:C43" xr:uid="{3A3A890D-49EE-4770-A722-1CC87E690383}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3446A694-FFC3-4055-806C-88612CAD91BE}" name="Species" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{588DB093-7048-463E-BBC0-CA002D126DBC}" name="dCMP/dUMP Hmase" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{1C098997-A581-4F89-97B2-A476215468FF}" name="TS" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3446A694-FFC3-4055-806C-88612CAD91BE}" name="Species" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{588DB093-7048-463E-BBC0-CA002D126DBC}" name="dCMP/dUMP Hmase" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{1C098997-A581-4F89-97B2-A476215468FF}" name="TS" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4213F5E3-07B6-42EB-A42D-397534729087}" name="Table3" displayName="Table3" ref="A1:C82" totalsRowShown="0" headerRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4213F5E3-07B6-42EB-A42D-397534729087}" name="Table3" displayName="Table3" ref="A1:C82" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:C82" xr:uid="{4213F5E3-07B6-42EB-A42D-397534729087}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7F451A82-DC65-42A2-B88B-7B7994177647}" name="Species" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{66150FF0-0EE5-4F8C-AA31-89F4388A94DD}" name="Aat 1" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{86ED9663-004B-4963-A0EA-3CC7F284165A}" name="Aat 2" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{7F451A82-DC65-42A2-B88B-7B7994177647}" name="Species" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{66150FF0-0EE5-4F8C-AA31-89F4388A94DD}" name="Aat 1" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{86ED9663-004B-4963-A0EA-3CC7F284165A}" name="Aat 2" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4232,7 +4201,7 @@
   <autoFilter ref="A1:C15" xr:uid="{35953585-8BCC-43F3-B2EC-A4C93FD77ADA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6D15AC7D-604C-4694-9F41-1B658DA63A6D}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{DE3EDC77-4B78-4B56-AA56-6565DF147FC8}" name="Accession" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DE3EDC77-4B78-4B56-AA56-6565DF147FC8}" name="Accession" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{BD7ECED3-37F7-4FEC-B10A-4021C937310A}" name="Phage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4240,15 +4209,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FF010DBD-D1D4-442F-9E30-A2BC819FC95E}" name="Table6" displayName="Table6" ref="A1:F35" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FF010DBD-D1D4-442F-9E30-A2BC819FC95E}" name="Table6" displayName="Table6" ref="A1:F35" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:F35" xr:uid="{FF010DBD-D1D4-442F-9E30-A2BC819FC95E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{91593A0B-30A7-44DB-A322-B9853D94D392}" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{021D26FB-E448-4F6E-A9B8-FCD8A632A44E}" name="Phage" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{2A7E169F-E074-4DB6-B8B7-DA3BDC4EBE6D}" name="Modification" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{93D3F28D-0F70-4EAE-AB08-D0F5EC03A79C}" name="Accession" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{BF63045D-E6B3-41A5-B46B-CD27C31CBF47}" name="GeneProduct" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{BA849627-EAD6-4C34-B923-85DF0C54D911}" name="FromHost" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{91593A0B-30A7-44DB-A322-B9853D94D392}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{021D26FB-E448-4F6E-A9B8-FCD8A632A44E}" name="Phage" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{2A7E169F-E074-4DB6-B8B7-DA3BDC4EBE6D}" name="Modification" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{93D3F28D-0F70-4EAE-AB08-D0F5EC03A79C}" name="Accession" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{BF63045D-E6B3-41A5-B46B-CD27C31CBF47}" name="GeneProduct" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BA849627-EAD6-4C34-B923-85DF0C54D911}" name="FromHost" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4573,8 +4542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CFBFFF-D98C-46CE-BC5D-1A3986B5B44F}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4752,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DF88C9-F77D-413A-A818-EF11C4BBBAF8}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4765,13 +4734,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>270</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -4779,406 +4748,406 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="C2" s="5">
+        <v>166559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="9">
-        <v>166559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="5">
+        <v>164093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="C3" s="9">
-        <v>164093</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="5">
+        <v>166487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="9">
-        <v>166487</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="5">
+        <v>169176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="C5" s="9">
-        <v>169176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="5">
+        <v>167029</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C6" s="9">
-        <v>167029</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="5">
+        <v>166964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C7" s="9">
-        <v>166964</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="C8" s="5">
+        <v>164309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C8" s="9">
-        <v>164309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="C9" s="5">
+        <v>177643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="C9" s="9">
-        <v>177643</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="5">
+        <v>171269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C10" s="9">
-        <v>171269</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="C11" s="5">
+        <v>169031</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="9">
-        <v>169031</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C12" s="5">
+        <v>168968</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="C12" s="9">
-        <v>168968</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="C13" s="5">
+        <v>175437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C13" s="9">
-        <v>175437</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="5">
+        <v>168896</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="9">
-        <v>168896</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="C15" s="5">
+        <v>172253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="C15" s="9">
-        <v>172253</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="C16" s="5">
+        <v>168676</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="C16" s="9">
+      <c r="B17" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C17" s="5">
+        <v>168724</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="5">
         <v>168676</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="C17" s="9">
-        <v>168724</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="C18" s="9">
-        <v>168676</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="C19" s="5">
+        <v>167559</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C19" s="9">
-        <v>167559</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="C20" s="5">
+        <v>168695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C20" s="9">
-        <v>168695</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="5">
+        <v>171207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="C21" s="9">
-        <v>171207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="8" t="s">
+      <c r="B22" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="C22" s="5">
+        <v>163469</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C22" s="9">
-        <v>163469</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="C23" s="5">
+        <v>174432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="C23" s="9">
-        <v>174432</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="C24" s="5">
+        <v>171175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C24" s="9">
-        <v>171175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="8" t="s">
+      <c r="B25" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="5">
+        <v>172075</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C25" s="9">
-        <v>172075</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="5">
+        <v>172450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="C26" s="9">
-        <v>172450</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="C27" s="5">
+        <v>168893</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="C27" s="9">
-        <v>168893</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="8" t="s">
+      <c r="B28" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="5">
+        <v>170740</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="C28" s="9">
-        <v>170740</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>315</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="5">
+        <v>169744</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C29" s="9">
-        <v>169744</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C30" s="9">
+      <c r="C30" s="5">
         <v>162101</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B31" t="s">
-        <v>452</v>
-      </c>
-      <c r="C31" s="12">
+        <v>451</v>
+      </c>
+      <c r="C31" s="8">
         <v>168908</v>
       </c>
       <c r="D31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B32" t="s">
-        <v>451</v>
-      </c>
-      <c r="C32" s="12">
+        <v>450</v>
+      </c>
+      <c r="C32" s="8">
         <v>168903</v>
       </c>
       <c r="D32" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B33" t="s">
-        <v>453</v>
-      </c>
-      <c r="C33" s="12">
+        <v>452</v>
+      </c>
+      <c r="C33" s="8">
         <v>174432</v>
       </c>
       <c r="D33" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B34" t="s">
-        <v>454</v>
-      </c>
-      <c r="C34" s="12">
+        <v>453</v>
+      </c>
+      <c r="C34" s="8">
         <v>63971</v>
       </c>
       <c r="D34" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B35" t="s">
-        <v>455</v>
-      </c>
-      <c r="C35" s="12">
+        <v>454</v>
+      </c>
+      <c r="C35" s="8">
         <v>63971</v>
       </c>
       <c r="D35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B36" t="s">
+        <v>455</v>
+      </c>
+      <c r="C36" s="8">
+        <v>212807</v>
+      </c>
+      <c r="D36" t="s">
         <v>456</v>
-      </c>
-      <c r="C36" s="12">
-        <v>212807</v>
-      </c>
-      <c r="D36" t="s">
-        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -6250,355 +6219,355 @@
       <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C45" s="7"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B46" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="C45" s="11"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="C46" s="11"/>
+      <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C47" s="7"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C48" s="7"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C49" s="7"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C51" s="7"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C52" s="7"/>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C53" s="7"/>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C54" s="7"/>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C55" s="7"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C56" s="7"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C57" s="7"/>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C58" s="7"/>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C59" s="7"/>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C60" s="7"/>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C61" s="7"/>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C62" s="7"/>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C63" s="7"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C64" s="7"/>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C66" s="7"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C67" s="7"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C68" s="7"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C69" s="7"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C70" s="7"/>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C71" s="7"/>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C72" s="7"/>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C73" s="7"/>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C76" s="7"/>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C77" s="7"/>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C78" s="7"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C79" s="7"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="B81" s="7" t="s">
+      <c r="B82" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="C81" s="7"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="C82" s="11"/>
+      <c r="C82" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6623,163 +6592,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>458</v>
+      <c r="C1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B6" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>476</v>
-      </c>
-      <c r="C4" s="13" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="15" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="14" t="s">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>477</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="20" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>478</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>479</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="14" t="s">
-        <v>470</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="14" t="s">
-        <v>471</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="20" t="s">
-        <v>473</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6801,694 +6770,693 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="15" style="16" customWidth="1"/>
-    <col min="6" max="6" width="12" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="16" t="s">
+      <c r="A1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" t="s">
         <v>458</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>459</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C2" t="s">
         <v>460</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="D2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C6" t="s">
+        <v>460</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" t="s">
+        <v>466</v>
+      </c>
+      <c r="C7" t="s">
+        <v>460</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B8" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" t="s">
+        <v>460</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" t="s">
+        <v>460</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B10" t="s">
+        <v>466</v>
+      </c>
+      <c r="C10" t="s">
+        <v>460</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B11" t="s">
+        <v>466</v>
+      </c>
+      <c r="C11" t="s">
+        <v>460</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C12" t="s">
+        <v>460</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" t="s">
+        <v>467</v>
+      </c>
+      <c r="C13" t="s">
+        <v>461</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="F13" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B14" t="s">
         <v>467</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C14" t="s">
         <v>461</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>397</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="14" t="s">
+      <c r="D14" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="F14" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B15" t="s">
         <v>467</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C15" t="s">
         <v>461</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="14" t="s">
+      <c r="D15" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="F15" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B16" t="s">
         <v>467</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C16" t="s">
         <v>461</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>406</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
+      <c r="D16" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="F16" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17" t="s">
         <v>467</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C17" t="s">
         <v>461</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="D17" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B18" t="s">
         <v>467</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C18" t="s">
         <v>461</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>415</v>
-      </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="18" t="s">
+      <c r="D18" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="14" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B19" t="s">
+        <v>467</v>
+      </c>
+      <c r="C19" t="s">
+        <v>461</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B20" t="s">
+        <v>467</v>
+      </c>
+      <c r="C20" t="s">
+        <v>461</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B21" t="s">
+        <v>467</v>
+      </c>
+      <c r="C21" t="s">
+        <v>461</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B22" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B23" t="s">
+        <v>467</v>
+      </c>
+      <c r="C23" t="s">
+        <v>461</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B24" t="s">
+        <v>468</v>
+      </c>
+      <c r="C24" t="s">
+        <v>462</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B25" t="s">
+        <v>468</v>
+      </c>
+      <c r="C25" t="s">
+        <v>462</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B26" t="s">
+        <v>468</v>
+      </c>
+      <c r="C26" t="s">
+        <v>462</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B27" t="s">
+        <v>468</v>
+      </c>
+      <c r="C27" t="s">
+        <v>462</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B28" t="s">
+        <v>468</v>
+      </c>
+      <c r="C28" t="s">
+        <v>462</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C29" t="s">
+        <v>462</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="F29" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B30" t="s">
+        <v>468</v>
+      </c>
+      <c r="C30" t="s">
+        <v>462</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="F30" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B31" t="s">
+        <v>468</v>
+      </c>
+      <c r="C31" t="s">
+        <v>462</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>430</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="F31" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B32" t="s">
+        <v>468</v>
+      </c>
+      <c r="C32" t="s">
+        <v>462</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>435</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="F32" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B33" t="s">
+        <v>468</v>
+      </c>
+      <c r="C33" t="s">
+        <v>462</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>440</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>467</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>461</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="F33" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B34" t="s">
         <v>468</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C34" t="s">
         <v>462</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="D34" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" t="s">
         <v>468</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C35" t="s">
         <v>462</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>408</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>406</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>416</v>
-      </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="18" t="s">
+      <c r="D35" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>465</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
-        <v>418</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>431</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>436</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="14" t="s">
-        <v>438</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>441</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>468</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>462</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>444</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>396</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14" t="s">
-        <v>406</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>410</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="15" t="s">
-        <v>414</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>417</v>
-      </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="18" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="14" t="s">
-        <v>418</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="14" t="s">
-        <v>428</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>429</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="14" t="s">
-        <v>433</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>437</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>434</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="14" t="s">
-        <v>438</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>442</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>439</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="19" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="14" t="s">
-        <v>443</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>469</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>463</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -7500,6 +7468,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a2f89840-a7cc-4376-9980-06283c9d5b42" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37aec0f5-327e-4afa-91d9-267e84b4b045">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FC3620CFC7FEF4F8C7581EBFDBDE910" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dad35cf49c4622e1a297011be7d8f910">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="37aec0f5-327e-4afa-91d9-267e84b4b045" xmlns:ns3="a2f89840-a7cc-4376-9980-06283c9d5b42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24223c3cf2bd64e6723cbf83261c9ca2" ns2:_="" ns3:_="">
     <xsd:import namespace="37aec0f5-327e-4afa-91d9-267e84b4b045"/>
@@ -7754,17 +7733,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a2f89840-a7cc-4376-9980-06283c9d5b42" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="37aec0f5-327e-4afa-91d9-267e84b4b045">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7775,6 +7743,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F2C2ED-48BC-4EF7-B2A2-A366FB9973E2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a2f89840-a7cc-4376-9980-06283c9d5b42"/>
+    <ds:schemaRef ds:uri="37aec0f5-327e-4afa-91d9-267e84b4b045"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D729B990-EC3B-4AEC-9113-47632DD276AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7793,17 +7772,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F2C2ED-48BC-4EF7-B2A2-A366FB9973E2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a2f89840-a7cc-4376-9980-06283c9d5b42"/>
-    <ds:schemaRef ds:uri="37aec0f5-327e-4afa-91d9-267e84b4b045"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D78DB7D3-AC2A-4D00-8BFC-40E1E9681004}">
   <ds:schemaRefs>

</xml_diff>